<commit_message>
Curation WP5166 WP5169 WP5173 WP5190
- Split up list comprehensions
- Added space stripper for numerical values regex match
- Syntax is valid
</commit_message>
<xml_diff>
--- a/ValidateData/kinetic data_WP5169.xlsx
+++ b/ValidateData/kinetic data_WP5169.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="105">
   <si>
     <t xml:space="preserve">EnzymePW</t>
   </si>
@@ -73,7 +73,7 @@
     <t xml:space="preserve">Database</t>
   </si>
   <si>
-    <t xml:space="preserve">ALAS</t>
+    <t xml:space="preserve">ALAS2</t>
   </si>
   <si>
     <t xml:space="preserve">Delta-aminolevulinate synthase </t>
@@ -82,6 +82,9 @@
     <t xml:space="preserve">2.3.1.37</t>
   </si>
   <si>
+    <t xml:space="preserve">P22557</t>
+  </si>
+  <si>
     <t xml:space="preserve">-</t>
   </si>
   <si>
@@ -95,6 +98,9 @@
   </si>
   <si>
     <t xml:space="preserve">7.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“ usually only one isoform of bacterial ALAS proteins, mammals carry two different ALAS isoforms, one of them fulfilling a housekeeping function (ALAS1) and the other sustaining high levels of heme biosynthesis in erythrocytes (ALAS2); PMID: 2347585”</t>
   </si>
   <si>
     <t xml:space="preserve">Homo sapiens</t>
@@ -518,8 +524,8 @@
   </sheetPr>
   <dimension ref="A1:Q19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:Q1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -534,7 +540,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="13.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="11" style="0" width="8.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="15.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="15.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="14.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="17" style="0" width="8.53"/>
   </cols>
@@ -606,41 +612,41 @@
         <v>20</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M2" s="0" t="n">
         <v>37</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="P2" s="0" t="n">
         <v>20506125</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -657,841 +663,841 @@
         <v>20</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M3" s="0" t="n">
         <v>37</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="O3" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="P3" s="0" t="n">
         <v>20506125</v>
       </c>
       <c r="Q3" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N4" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O4" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="P4" s="0" t="n">
         <v>23720291</v>
       </c>
       <c r="Q4" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N5" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O5" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="P5" s="0" t="n">
         <v>23720291</v>
       </c>
       <c r="Q5" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N6" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O6" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="P6" s="0" t="n">
         <v>30594473</v>
       </c>
       <c r="Q6" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L7" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M7" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N7" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O7" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="P7" s="0" t="n">
         <v>30594473</v>
       </c>
       <c r="Q7" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L8" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M8" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N8" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O8" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="P8" s="0" t="n">
         <v>30594473</v>
       </c>
       <c r="Q8" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>20</v>
+        <v>68</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M9" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N9" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O9" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="P9" s="0" t="n">
         <v>10692079</v>
       </c>
       <c r="Q9" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>20</v>
+        <v>68</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>20</v>
+        <v>72</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L10" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M10" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N10" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O10" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="P10" s="0" t="n">
         <v>31326287</v>
       </c>
       <c r="Q10" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>20</v>
+        <v>68</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>20</v>
+        <v>72</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K11" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M11" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N11" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O11" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="P11" s="0" t="n">
         <v>10692079</v>
       </c>
       <c r="Q11" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>20</v>
+        <v>68</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>20</v>
+        <v>72</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L12" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M12" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N12" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O12" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="P12" s="0" t="n">
         <v>31326287</v>
       </c>
       <c r="Q12" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>20</v>
+        <v>68</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>20</v>
+        <v>72</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L13" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M13" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N13" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O13" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="P13" s="0" t="n">
         <v>10692079</v>
       </c>
       <c r="Q13" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>20</v>
+        <v>68</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>20</v>
+        <v>72</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L14" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M14" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N14" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O14" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="P14" s="0" t="n">
         <v>31326287</v>
       </c>
       <c r="Q14" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>20</v>
+        <v>68</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L15" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="M15" s="0" t="n">
         <v>37</v>
       </c>
       <c r="N15" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O15" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="P15" s="0" t="n">
         <v>10692079</v>
       </c>
       <c r="Q15" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>20</v>
+        <v>68</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L16" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M16" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N16" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O16" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="P16" s="0" t="n">
         <v>31326287</v>
       </c>
       <c r="Q16" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K17" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L17" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M17" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N17" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O17" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="P17" s="0" t="n">
         <v>30594473</v>
       </c>
       <c r="Q17" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K18" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L18" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M18" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N18" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O18" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="P18" s="0" t="n">
         <v>30594473</v>
       </c>
       <c r="Q18" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L19" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M19" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="N19" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O19" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="P19" s="0" t="n">
         <v>30594473</v>
       </c>
       <c r="Q19" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>